<commit_message>
funciona todo, haciendo el script/ jueves
</commit_message>
<xml_diff>
--- a/kafka-mates-datos/reporte.xlsx
+++ b/kafka-mates-datos/reporte.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Productos" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Ventas" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Estadísticas" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,14 +437,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>identificador</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>categoria</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>identificador</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>producto</t>
@@ -459,30 +458,90 @@
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>precioPromocionado</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>promocionTimestamp</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mate premium</t>
+          <t>02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>accesorios</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>matera</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E2" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1738266760087</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>01</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mate</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>mate torpedo</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1738269208022</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mate</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>mate imperial</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>18</v>
-      </c>
-      <c r="E2" t="n">
-        <v>18</v>
+      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1738269208022</v>
       </c>
     </row>
   </sheetData>
@@ -496,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,24 +586,29 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>precioConImpuesto</t>
+          <t>precioConImpuesto_x</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>precioPromocionado</t>
+          <t>precioPromocionado_x</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>monto</t>
+          <t>precioConImpuesto_y</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>precioPromocionado_y</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mate premium</t>
+          <t>mate</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -554,61 +618,55 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mate imperial</t>
+          <t>mate torpedo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F2" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G2" t="n">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="H2" t="n">
+        <v>24</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>monto</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>mate premium</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>18</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>accesorios</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>matera</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3" t="n">
+        <v>21.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>